<commit_message>
Add code and docs
</commit_message>
<xml_diff>
--- a/reports/Output_Report.xlsx
+++ b/reports/Output_Report.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="79">
   <si>
     <t>Title</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>Baseline</t>
+  </si>
+  <si>
+    <t>Logistic</t>
   </si>
   <si>
     <t>KNN3</t>
@@ -2480,31 +2483,31 @@
     </row>
     <row r="2" spans="1:24">
       <c r="A2" s="2" t="n">
-        <v>561663</v>
+        <v>477829</v>
       </c>
       <c r="B2" t="n">
-        <v>43.09</v>
+        <v>38.33</v>
       </c>
       <c r="C2" t="n">
-        <v>45.43</v>
+        <v>38.65</v>
       </c>
       <c r="D2" t="n">
-        <v>43.01</v>
+        <v>38.22</v>
       </c>
       <c r="E2" t="n">
-        <v>45.25</v>
+        <v>38.42</v>
       </c>
       <c r="F2" t="n">
-        <v>11738415</v>
+        <v>4625616</v>
       </c>
       <c r="G2" t="n">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="H2" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I2" t="n">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="J2" t="n">
         <v>4</v>
@@ -2513,22 +2516,22 @@
         <v>1</v>
       </c>
       <c r="L2" t="n">
-        <v>0.3938204637296789</v>
+        <v>-0.8617317476237206</v>
       </c>
       <c r="M2" t="n">
-        <v>1.701558387044675</v>
+        <v>3.468767610724833</v>
       </c>
       <c r="N2" t="n">
-        <v>2.420000000000002</v>
+        <v>0.4299999999999997</v>
       </c>
       <c r="O2" t="n">
-        <v>2.240000000000002</v>
+        <v>0.2000000000000028</v>
       </c>
       <c r="P2" t="n">
-        <v>0.1799999999999997</v>
+        <v>0.2299999999999969</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.054287045666356</v>
+        <v>0.003395142334813306</v>
       </c>
       <c r="R2" t="b">
         <v>1</v>
@@ -2537,16 +2540,16 @@
         <v>1</v>
       </c>
       <c r="T2" t="n">
-        <v>46.05800000000006</v>
+        <v>38.59700000000003</v>
       </c>
       <c r="U2" t="n">
-        <v>48.038</v>
+        <v>38.51099999999998</v>
       </c>
       <c r="V2" t="n">
-        <v>49.79680000000002</v>
+        <v>39.29139999999997</v>
       </c>
       <c r="W2" t="n">
-        <v>1.116672352508174</v>
+        <v>0.2722393904530523</v>
       </c>
       <c r="X2" t="n">
         <v>0</v>
@@ -2554,73 +2557,73 @@
     </row>
     <row r="3" spans="1:24">
       <c r="A3" s="2" t="n">
-        <v>562220</v>
+        <v>477914</v>
       </c>
       <c r="B3" t="n">
-        <v>45.23</v>
+        <v>38.48</v>
       </c>
       <c r="C3" t="n">
-        <v>45.3718</v>
+        <v>38.94</v>
       </c>
       <c r="D3" t="n">
-        <v>44.78</v>
+        <v>38.47</v>
       </c>
       <c r="E3" t="n">
-        <v>44.95</v>
+        <v>38.6</v>
       </c>
       <c r="F3" t="n">
-        <v>6969256</v>
+        <v>6633668</v>
       </c>
       <c r="G3" t="n">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="H3" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I3" t="n">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>0.2949012456943941</v>
+        <v>-0.3927770088050948</v>
       </c>
       <c r="M3" t="n">
-        <v>1.879038558168715</v>
+        <v>1.083033712456359</v>
       </c>
       <c r="N3" t="n">
-        <v>0.5917999999999992</v>
+        <v>0.4699999999999989</v>
       </c>
       <c r="O3" t="n">
-        <v>0.1700000000000017</v>
+        <v>0.1300000000000026</v>
       </c>
       <c r="P3" t="n">
-        <v>0.4217999999999975</v>
+        <v>0.3399999999999963</v>
       </c>
       <c r="Q3" t="n">
-        <v>-0.006629834254143541</v>
+        <v>0.004685059864653729</v>
       </c>
       <c r="R3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S3" t="b">
         <v>1</v>
       </c>
       <c r="T3" t="n">
-        <v>45.67200000000005</v>
+        <v>38.53700000000003</v>
       </c>
       <c r="U3" t="n">
-        <v>47.76350000000001</v>
+        <v>38.50399999999998</v>
       </c>
       <c r="V3" t="n">
-        <v>49.72000000000002</v>
+        <v>39.24759999999998</v>
       </c>
       <c r="W3" t="n">
-        <v>1.017131821769509</v>
+        <v>0.1637506815688019</v>
       </c>
       <c r="X3" t="n">
         <v>0</v>
@@ -2628,55 +2631,55 @@
     </row>
     <row r="4" spans="1:24">
       <c r="A4" s="2" t="n">
-        <v>562614</v>
+        <v>478690</v>
       </c>
       <c r="B4" t="n">
-        <v>44.53</v>
+        <v>38.63</v>
       </c>
       <c r="C4" t="n">
-        <v>44.85</v>
+        <v>38.77</v>
       </c>
       <c r="D4" t="n">
-        <v>44.38</v>
+        <v>38.075</v>
       </c>
       <c r="E4" t="n">
-        <v>44.56</v>
+        <v>38.22</v>
       </c>
       <c r="F4" t="n">
-        <v>5195211</v>
+        <v>6828535</v>
       </c>
       <c r="G4" t="n">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="H4" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I4" t="n">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="J4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.3142011895447324</v>
+        <v>-1.677697914705399</v>
       </c>
       <c r="M4" t="n">
-        <v>1.426409302233204</v>
+        <v>2.390799103041162</v>
       </c>
       <c r="N4" t="n">
-        <v>0.4699999999999989</v>
+        <v>0.6950000000000003</v>
       </c>
       <c r="O4" t="n">
-        <v>0.1799999999999997</v>
+        <v>0.144999999999996</v>
       </c>
       <c r="P4" t="n">
-        <v>0.2899999999999991</v>
+        <v>0.5500000000000043</v>
       </c>
       <c r="Q4" t="n">
-        <v>-0.008676307007786432</v>
+        <v>-0.009844559585492241</v>
       </c>
       <c r="R4" t="b">
         <v>0</v>
@@ -2685,16 +2688,16 @@
         <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>45.27600000000005</v>
+        <v>38.41500000000003</v>
       </c>
       <c r="U4" t="n">
-        <v>47.43850000000001</v>
+        <v>38.47849999999998</v>
       </c>
       <c r="V4" t="n">
-        <v>49.61800000000002</v>
+        <v>39.20019999999997</v>
       </c>
       <c r="W4" t="n">
-        <v>0.9667545116074326</v>
+        <v>0.1428785698215396</v>
       </c>
       <c r="X4" t="n">
         <v>0</v>
@@ -2702,73 +2705,73 @@
     </row>
     <row r="5" spans="1:24">
       <c r="A5" s="2" t="n">
-        <v>563204</v>
+        <v>479104</v>
       </c>
       <c r="B5" t="n">
-        <v>44.54</v>
+        <v>38.3</v>
       </c>
       <c r="C5" t="n">
-        <v>44.765</v>
+        <v>38.51</v>
       </c>
       <c r="D5" t="n">
-        <v>43.89</v>
+        <v>38.11</v>
       </c>
       <c r="E5" t="n">
-        <v>44.32</v>
+        <v>38.31</v>
       </c>
       <c r="F5" t="n">
-        <v>5472629</v>
+        <v>7050816</v>
       </c>
       <c r="G5" t="n">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="H5" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I5" t="n">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="J5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>0.4721720435395593</v>
+        <v>-0.72740105857175</v>
       </c>
       <c r="M5" t="n">
-        <v>1.942639584281685</v>
+        <v>2.058535432344228</v>
       </c>
       <c r="N5" t="n">
-        <v>0.875</v>
+        <v>0.3999999999999986</v>
       </c>
       <c r="O5" t="n">
-        <v>0.4299999999999997</v>
+        <v>0.2000000000000028</v>
       </c>
       <c r="P5" t="n">
-        <v>0.4450000000000003</v>
+        <v>0.1999999999999957</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.005385996409335791</v>
+        <v>0.002354788069073965</v>
       </c>
       <c r="R5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5" t="b">
         <v>0</v>
       </c>
       <c r="T5" t="n">
-        <v>44.86700000000005</v>
+        <v>38.36400000000004</v>
       </c>
       <c r="U5" t="n">
-        <v>47.13200000000001</v>
+        <v>38.49049999999998</v>
       </c>
       <c r="V5" t="n">
-        <v>49.54380000000002</v>
+        <v>39.14299999999997</v>
       </c>
       <c r="W5" t="n">
-        <v>0.8567713480598024</v>
+        <v>0.1429285535802204</v>
       </c>
       <c r="X5" t="n">
         <v>0</v>
@@ -2776,55 +2779,55 @@
     </row>
     <row r="6" spans="1:24">
       <c r="A6" s="2" t="n">
-        <v>563647</v>
+        <v>479383</v>
       </c>
       <c r="B6" t="n">
-        <v>44.54</v>
+        <v>38.33</v>
       </c>
       <c r="C6" t="n">
-        <v>44.94</v>
+        <v>38.87</v>
       </c>
       <c r="D6" t="n">
-        <v>44.43</v>
+        <v>38.25</v>
       </c>
       <c r="E6" t="n">
-        <v>44.74</v>
+        <v>38.41</v>
       </c>
       <c r="F6" t="n">
-        <v>3799621</v>
+        <v>10445631</v>
       </c>
       <c r="G6" t="n">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="H6" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I6" t="n">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="J6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.8669952992645312</v>
+        <v>-0.3684254738407358</v>
       </c>
       <c r="M6" t="n">
-        <v>1.670433078337801</v>
+        <v>0.9028680566397101</v>
       </c>
       <c r="N6" t="n">
-        <v>0.509999999999998</v>
+        <v>0.6199999999999974</v>
       </c>
       <c r="O6" t="n">
-        <v>0.3100000000000023</v>
+        <v>0.1599999999999966</v>
       </c>
       <c r="P6" t="n">
-        <v>0.1999999999999957</v>
+        <v>0.4600000000000009</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.009476534296029016</v>
+        <v>0.002610284521012751</v>
       </c>
       <c r="R6" t="b">
         <v>1</v>
@@ -2833,16 +2836,16 @@
         <v>1</v>
       </c>
       <c r="T6" t="n">
-        <v>44.73800000000006</v>
+        <v>38.31200000000004</v>
       </c>
       <c r="U6" t="n">
-        <v>46.84150000000001</v>
+        <v>38.53099999999998</v>
       </c>
       <c r="V6" t="n">
-        <v>49.47000000000002</v>
+        <v>39.11099999999998</v>
       </c>
       <c r="W6" t="n">
-        <v>0.7688457644566253</v>
+        <v>0.1322695660203158</v>
       </c>
       <c r="X6" t="n">
         <v>0</v>
@@ -2850,55 +2853,55 @@
     </row>
     <row r="7" spans="1:24">
       <c r="A7" s="2" t="n">
-        <v>564452</v>
+        <v>479880</v>
       </c>
       <c r="B7" t="n">
-        <v>44.85</v>
+        <v>38.6334</v>
       </c>
       <c r="C7" t="n">
-        <v>45.47</v>
+        <v>39.08</v>
       </c>
       <c r="D7" t="n">
-        <v>44.65</v>
+        <v>38.34</v>
       </c>
       <c r="E7" t="n">
-        <v>45.31</v>
+        <v>39.05</v>
       </c>
       <c r="F7" t="n">
-        <v>4569439</v>
+        <v>9677316</v>
       </c>
       <c r="G7" t="n">
         <v>2017</v>
       </c>
       <c r="H7" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="J7" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>-2.026008636954774</v>
+        <v>-0.001535312481727814</v>
       </c>
       <c r="M7" t="n">
-        <v>3.245616174613259</v>
+        <v>0.8252654646741249</v>
       </c>
       <c r="N7" t="n">
-        <v>0.8200000000000003</v>
+        <v>0.7399999999999949</v>
       </c>
       <c r="O7" t="n">
-        <v>0.6600000000000037</v>
+        <v>0.7099999999999937</v>
       </c>
       <c r="P7" t="n">
-        <v>0.1599999999999966</v>
+        <v>0.03000000000000114</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.01274027715690651</v>
+        <v>0.01666232751887531</v>
       </c>
       <c r="R7" t="b">
         <v>1</v>
@@ -2907,16 +2910,16 @@
         <v>1</v>
       </c>
       <c r="T7" t="n">
-        <v>44.71400000000006</v>
+        <v>38.40700000000004</v>
       </c>
       <c r="U7" t="n">
-        <v>46.56700000000002</v>
+        <v>38.58849999999997</v>
       </c>
       <c r="V7" t="n">
-        <v>49.39680000000002</v>
+        <v>39.07719999999998</v>
       </c>
       <c r="W7" t="n">
-        <v>0.8132123251115551</v>
+        <v>0.2828090387185769</v>
       </c>
       <c r="X7" t="n">
         <v>0</v>
@@ -2924,73 +2927,73 @@
     </row>
     <row r="8" spans="1:24">
       <c r="A8" s="2" t="n">
-        <v>564990</v>
+        <v>480634</v>
       </c>
       <c r="B8" t="n">
-        <v>44.79</v>
+        <v>39.06</v>
       </c>
       <c r="C8" t="n">
-        <v>45.28</v>
+        <v>39.725</v>
       </c>
       <c r="D8" t="n">
-        <v>43.84</v>
+        <v>39.06</v>
       </c>
       <c r="E8" t="n">
-        <v>43.92</v>
+        <v>39.36</v>
       </c>
       <c r="F8" t="n">
-        <v>8512885</v>
+        <v>22644542</v>
       </c>
       <c r="G8" t="n">
         <v>2017</v>
       </c>
       <c r="H8" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.7118688280795344</v>
+        <v>-0.4257525001867117</v>
       </c>
       <c r="M8" t="n">
-        <v>3.379955005532874</v>
+        <v>2.072082611624386</v>
       </c>
       <c r="N8" t="n">
-        <v>1.439999999999998</v>
+        <v>0.6649999999999991</v>
       </c>
       <c r="O8" t="n">
-        <v>0.07999999999999829</v>
+        <v>0.2999999999999972</v>
       </c>
       <c r="P8" t="n">
-        <v>1.359999999999999</v>
+        <v>0.365000000000002</v>
       </c>
       <c r="Q8" t="n">
-        <v>-0.03067755462370336</v>
+        <v>0.007938540332906641</v>
       </c>
       <c r="R8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T8" t="n">
-        <v>44.53500000000006</v>
+        <v>38.50900000000004</v>
       </c>
       <c r="U8" t="n">
-        <v>46.23400000000002</v>
+        <v>38.63499999999998</v>
       </c>
       <c r="V8" t="n">
-        <v>49.30260000000002</v>
+        <v>39.05439999999997</v>
       </c>
       <c r="W8" t="n">
-        <v>0.5013125628919739</v>
+        <v>0.4228812734427431</v>
       </c>
       <c r="X8" t="n">
         <v>0</v>
@@ -2998,73 +3001,73 @@
     </row>
     <row r="9" spans="1:24">
       <c r="A9" s="2" t="n">
-        <v>565558</v>
+        <v>481023</v>
       </c>
       <c r="B9" t="n">
-        <v>43.09</v>
+        <v>39.24</v>
       </c>
       <c r="C9" t="n">
-        <v>44.68</v>
+        <v>39.75</v>
       </c>
       <c r="D9" t="n">
-        <v>42.6066</v>
+        <v>38.98</v>
       </c>
       <c r="E9" t="n">
-        <v>44.31</v>
+        <v>39.7</v>
       </c>
       <c r="F9" t="n">
-        <v>8796667</v>
+        <v>12080148</v>
       </c>
       <c r="G9" t="n">
         <v>2017</v>
       </c>
       <c r="H9" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K9" t="n">
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>-3.041616585233114</v>
+        <v>-1.007884373412614</v>
       </c>
       <c r="M9" t="n">
-        <v>5.248832833733428</v>
+        <v>1.58763190549809</v>
       </c>
       <c r="N9" t="n">
-        <v>2.073399999999999</v>
+        <v>0.7700000000000031</v>
       </c>
       <c r="O9" t="n">
-        <v>1.703400000000002</v>
+        <v>0.720000000000006</v>
       </c>
       <c r="P9" t="n">
-        <v>0.3699999999999974</v>
+        <v>0.04999999999999716</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.008879781420765065</v>
+        <v>0.008638211382113958</v>
       </c>
       <c r="R9" t="b">
         <v>1</v>
       </c>
       <c r="S9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T9" t="n">
-        <v>44.42500000000005</v>
+        <v>38.66000000000004</v>
       </c>
       <c r="U9" t="n">
-        <v>45.94950000000001</v>
+        <v>38.69899999999998</v>
       </c>
       <c r="V9" t="n">
-        <v>49.21320000000001</v>
+        <v>39.04019999999997</v>
       </c>
       <c r="W9" t="n">
-        <v>0.4603518323226961</v>
+        <v>0.5707221824353857</v>
       </c>
       <c r="X9" t="n">
         <v>0</v>
@@ -3072,73 +3075,73 @@
     </row>
     <row r="10" spans="1:24">
       <c r="A10" s="2" t="n">
-        <v>565958</v>
+        <v>481465</v>
       </c>
       <c r="B10" t="n">
-        <v>44.19</v>
+        <v>39.7</v>
       </c>
       <c r="C10" t="n">
-        <v>44.625</v>
+        <v>40.99</v>
       </c>
       <c r="D10" t="n">
-        <v>43.5347</v>
+        <v>39.66</v>
       </c>
       <c r="E10" t="n">
-        <v>43.84</v>
+        <v>40.78</v>
       </c>
       <c r="F10" t="n">
-        <v>5095010</v>
+        <v>14628910</v>
       </c>
       <c r="G10" t="n">
         <v>2017</v>
       </c>
       <c r="H10" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10" t="n">
-        <v>-1.168213247738408</v>
+        <v>-0.08053302393734339</v>
       </c>
       <c r="M10" t="n">
-        <v>3.2686968335588</v>
+        <v>1.416439538366582</v>
       </c>
       <c r="N10" t="n">
-        <v>1.090299999999999</v>
+        <v>1.330000000000005</v>
       </c>
       <c r="O10" t="n">
-        <v>0.3053000000000026</v>
+        <v>1.120000000000005</v>
       </c>
       <c r="P10" t="n">
-        <v>0.7849999999999966</v>
+        <v>0.2100000000000009</v>
       </c>
       <c r="Q10" t="n">
-        <v>-0.01060708643647035</v>
+        <v>0.02720403022670026</v>
       </c>
       <c r="R10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T10" t="n">
-        <v>44.41200000000006</v>
+        <v>38.91400000000003</v>
       </c>
       <c r="U10" t="n">
-        <v>45.67150000000002</v>
+        <v>38.81399999999998</v>
       </c>
       <c r="V10" t="n">
-        <v>49.12000000000002</v>
+        <v>39.05199999999997</v>
       </c>
       <c r="W10" t="n">
-        <v>0.5036675018104987</v>
+        <v>0.9241830369111451</v>
       </c>
       <c r="X10" t="n">
         <v>0</v>
@@ -3146,73 +3149,73 @@
     </row>
     <row r="11" spans="1:24">
       <c r="A11" s="2" t="n">
-        <v>566066</v>
+        <v>481988</v>
       </c>
       <c r="B11" t="n">
-        <v>43.81</v>
+        <v>40.79</v>
       </c>
       <c r="C11" t="n">
-        <v>44.11</v>
+        <v>41.06</v>
       </c>
       <c r="D11" t="n">
-        <v>43.49</v>
+        <v>40.62</v>
       </c>
       <c r="E11" t="n">
-        <v>43.6</v>
+        <v>40.74</v>
       </c>
       <c r="F11" t="n">
-        <v>4684643</v>
+        <v>10992496</v>
       </c>
       <c r="G11" t="n">
         <v>2017</v>
       </c>
       <c r="H11" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="J11" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
         <v>1</v>
       </c>
       <c r="L11" t="n">
-        <v>-0.1937241888917663</v>
+        <v>0.06830932649096508</v>
       </c>
       <c r="M11" t="n">
-        <v>0.4905499808765012</v>
+        <v>1.583589173644811</v>
       </c>
       <c r="N11" t="n">
-        <v>0.6199999999999974</v>
+        <v>0.4400000000000048</v>
       </c>
       <c r="O11" t="n">
-        <v>0.1099999999999994</v>
+        <v>0.1200000000000045</v>
       </c>
       <c r="P11" t="n">
-        <v>0.509999999999998</v>
+        <v>0.3200000000000003</v>
       </c>
       <c r="Q11" t="n">
-        <v>-0.005474452554744547</v>
+        <v>-0.0009808729769494873</v>
       </c>
       <c r="R11" t="b">
         <v>0</v>
       </c>
       <c r="S11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T11" t="n">
-        <v>44.48000000000006</v>
+        <v>39.15900000000003</v>
       </c>
       <c r="U11" t="n">
-        <v>45.42400000000002</v>
+        <v>38.91699999999999</v>
       </c>
       <c r="V11" t="n">
-        <v>49.00700000000002</v>
+        <v>39.06759999999997</v>
       </c>
       <c r="W11" t="n">
-        <v>0.5859018282784656</v>
+        <v>1.003251855574826</v>
       </c>
       <c r="X11" t="n">
         <v>0</v>
@@ -3220,55 +3223,55 @@
     </row>
     <row r="12" spans="1:24">
       <c r="A12" s="2" t="n">
-        <v>567055</v>
+        <v>482798</v>
       </c>
       <c r="B12" t="n">
-        <v>44.01</v>
+        <v>40.81</v>
       </c>
       <c r="C12" t="n">
-        <v>46.09</v>
+        <v>41.62</v>
       </c>
       <c r="D12" t="n">
-        <v>44</v>
+        <v>40.78</v>
       </c>
       <c r="E12" t="n">
-        <v>45.86</v>
+        <v>41.29</v>
       </c>
       <c r="F12" t="n">
-        <v>7921608</v>
+        <v>9256298</v>
       </c>
       <c r="G12" t="n">
         <v>2017</v>
       </c>
       <c r="H12" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I12" t="n">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>-0.8250281714622505</v>
+        <v>-1.048792289484141</v>
       </c>
       <c r="M12" t="n">
-        <v>4.495725369038267</v>
+        <v>3.180798099336217</v>
       </c>
       <c r="N12" t="n">
-        <v>2.090000000000003</v>
+        <v>0.8399999999999963</v>
       </c>
       <c r="O12" t="n">
-        <v>1.859999999999999</v>
+        <v>0.509999999999998</v>
       </c>
       <c r="P12" t="n">
-        <v>0.230000000000004</v>
+        <v>0.3299999999999983</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.05183486238532109</v>
+        <v>0.0135002454590083</v>
       </c>
       <c r="R12" t="b">
         <v>1</v>
@@ -3277,16 +3280,16 @@
         <v>1</v>
       </c>
       <c r="T12" t="n">
-        <v>44.54100000000006</v>
+        <v>39.44600000000003</v>
       </c>
       <c r="U12" t="n">
-        <v>45.29950000000002</v>
+        <v>39.02149999999998</v>
       </c>
       <c r="V12" t="n">
-        <v>48.93180000000002</v>
+        <v>39.08759999999997</v>
       </c>
       <c r="W12" t="n">
-        <v>0.8347140941943423</v>
+        <v>1.055633414004114</v>
       </c>
       <c r="X12" t="n">
         <v>0</v>
@@ -3294,73 +3297,73 @@
     </row>
     <row r="13" spans="1:24">
       <c r="A13" s="2" t="n">
-        <v>567285</v>
+        <v>483171</v>
       </c>
       <c r="B13" t="n">
-        <v>45.9</v>
+        <v>41.05</v>
       </c>
       <c r="C13" t="n">
-        <v>46.48</v>
+        <v>41.415</v>
       </c>
       <c r="D13" t="n">
-        <v>45.63</v>
+        <v>40.485</v>
       </c>
       <c r="E13" t="n">
-        <v>46.29</v>
+        <v>41.08</v>
       </c>
       <c r="F13" t="n">
-        <v>6325114</v>
+        <v>10699446</v>
       </c>
       <c r="G13" t="n">
         <v>2017</v>
       </c>
       <c r="H13" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="J13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K13" t="n">
         <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>-0.8039691003465332</v>
+        <v>-1.081260404628781</v>
       </c>
       <c r="M13" t="n">
-        <v>2.226723386985266</v>
+        <v>2.384555478068116</v>
       </c>
       <c r="N13" t="n">
-        <v>0.8499999999999943</v>
+        <v>0.9299999999999997</v>
       </c>
       <c r="O13" t="n">
-        <v>0.6599999999999966</v>
+        <v>0.5949999999999989</v>
       </c>
       <c r="P13" t="n">
-        <v>0.1899999999999977</v>
+        <v>0.3350000000000009</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.009376362843436459</v>
+        <v>-0.005085977234197125</v>
       </c>
       <c r="R13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S13" t="b">
         <v>1</v>
       </c>
       <c r="T13" t="n">
-        <v>44.67500000000006</v>
+        <v>39.69400000000003</v>
       </c>
       <c r="U13" t="n">
-        <v>45.17350000000001</v>
+        <v>39.11549999999998</v>
       </c>
       <c r="V13" t="n">
-        <v>48.85120000000002</v>
+        <v>39.11839999999997</v>
       </c>
       <c r="W13" t="n">
-        <v>1.076130634661132</v>
+        <v>0.8960256161304793</v>
       </c>
       <c r="X13" t="n">
         <v>0</v>
@@ -3368,73 +3371,73 @@
     </row>
     <row r="14" spans="1:24">
       <c r="A14" s="2" t="n">
-        <v>567852</v>
+        <v>483525</v>
       </c>
       <c r="B14" t="n">
-        <v>46.35</v>
+        <v>40.79</v>
       </c>
       <c r="C14" t="n">
-        <v>47.58</v>
+        <v>40.79</v>
       </c>
       <c r="D14" t="n">
-        <v>46.1</v>
+        <v>40.31</v>
       </c>
       <c r="E14" t="n">
-        <v>47</v>
+        <v>40.72</v>
       </c>
       <c r="F14" t="n">
-        <v>7288178</v>
+        <v>8633354</v>
       </c>
       <c r="G14" t="n">
         <v>2017</v>
       </c>
       <c r="H14" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I14" t="n">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="J14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K14" t="n">
         <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>-0.1163635890021571</v>
+        <v>0.09094838994896931</v>
       </c>
       <c r="M14" t="n">
-        <v>2.303720392268894</v>
+        <v>1.591254806103937</v>
       </c>
       <c r="N14" t="n">
-        <v>1.479999999999997</v>
+        <v>0.4799999999999969</v>
       </c>
       <c r="O14" t="n">
-        <v>0.8999999999999986</v>
+        <v>0.4099999999999966</v>
       </c>
       <c r="P14" t="n">
-        <v>0.5799999999999983</v>
+        <v>0.07000000000000028</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.01533808597969322</v>
+        <v>-0.008763388510223957</v>
       </c>
       <c r="R14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T14" t="n">
-        <v>44.91900000000006</v>
+        <v>39.94400000000003</v>
       </c>
       <c r="U14" t="n">
-        <v>45.09750000000001</v>
+        <v>39.17949999999998</v>
       </c>
       <c r="V14" t="n">
-        <v>48.78340000000002</v>
+        <v>39.14799999999997</v>
       </c>
       <c r="W14" t="n">
-        <v>1.375207343673756</v>
+        <v>0.7165160417571662</v>
       </c>
       <c r="X14" t="n">
         <v>0</v>
@@ -3442,73 +3445,73 @@
     </row>
     <row r="15" spans="1:24">
       <c r="A15" s="2" t="n">
-        <v>568132</v>
+        <v>484129</v>
       </c>
       <c r="B15" t="n">
-        <v>46.79</v>
+        <v>40.75</v>
       </c>
       <c r="C15" t="n">
-        <v>46.94</v>
+        <v>41.36</v>
       </c>
       <c r="D15" t="n">
-        <v>46.12</v>
+        <v>40.69</v>
       </c>
       <c r="E15" t="n">
-        <v>46.19</v>
+        <v>40.93</v>
       </c>
       <c r="F15" t="n">
-        <v>5360496</v>
+        <v>9533780</v>
       </c>
       <c r="G15" t="n">
         <v>2017</v>
       </c>
       <c r="H15" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I15" t="n">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="J15" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" t="n">
-        <v>-0.8343482630857607</v>
+        <v>-1.059414378414707</v>
       </c>
       <c r="M15" t="n">
-        <v>1.268600059201549</v>
+        <v>2.150889070549688</v>
       </c>
       <c r="N15" t="n">
-        <v>0.8200000000000003</v>
+        <v>0.6700000000000017</v>
       </c>
       <c r="O15" t="n">
-        <v>0.07000000000000028</v>
+        <v>0.240000000000002</v>
       </c>
       <c r="P15" t="n">
-        <v>0.75</v>
+        <v>0.4299999999999997</v>
       </c>
       <c r="Q15" t="n">
-        <v>-0.0172340425531915</v>
+        <v>0.005157170923379306</v>
       </c>
       <c r="R15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S15" t="b">
         <v>0</v>
       </c>
       <c r="T15" t="n">
-        <v>45.10600000000007</v>
+        <v>40.20600000000003</v>
       </c>
       <c r="U15" t="n">
-        <v>44.98650000000002</v>
+        <v>39.28499999999998</v>
       </c>
       <c r="V15" t="n">
-        <v>48.68200000000002</v>
+        <v>39.18559999999997</v>
       </c>
       <c r="W15" t="n">
-        <v>1.352620032522029</v>
+        <v>0.5061761409968094</v>
       </c>
       <c r="X15" t="n">
         <v>0</v>
@@ -3516,73 +3519,73 @@
     </row>
     <row r="16" spans="1:24">
       <c r="A16" s="2" t="n">
-        <v>569058</v>
+        <v>484770</v>
       </c>
       <c r="B16" t="n">
-        <v>45.3</v>
+        <v>40.67</v>
       </c>
       <c r="C16" t="n">
-        <v>46.04</v>
+        <v>41.04</v>
       </c>
       <c r="D16" t="n">
-        <v>45.19</v>
+        <v>40.53</v>
       </c>
       <c r="E16" t="n">
-        <v>46</v>
+        <v>40.9</v>
       </c>
       <c r="F16" t="n">
-        <v>14846236</v>
+        <v>8272727</v>
       </c>
       <c r="G16" t="n">
         <v>2017</v>
       </c>
       <c r="H16" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I16" t="n">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="J16" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16" t="n">
-        <v>0.5458522458772415</v>
+        <v>-1.053007754034981</v>
       </c>
       <c r="M16" t="n">
-        <v>4.181972094441937</v>
+        <v>3.11375082246881</v>
       </c>
       <c r="N16" t="n">
-        <v>0.8500000000000014</v>
+        <v>0.509999999999998</v>
       </c>
       <c r="O16" t="n">
-        <v>0.8100000000000023</v>
+        <v>0.3699999999999974</v>
       </c>
       <c r="P16" t="n">
-        <v>0.03999999999999915</v>
+        <v>0.1400000000000006</v>
       </c>
       <c r="Q16" t="n">
-        <v>-0.004113444468499594</v>
+        <v>-0.0007329587099926815</v>
       </c>
       <c r="R16" t="b">
         <v>0</v>
       </c>
       <c r="S16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T16" t="n">
-        <v>45.23200000000006</v>
+        <v>40.45500000000003</v>
       </c>
       <c r="U16" t="n">
-        <v>44.98500000000002</v>
+        <v>39.38349999999998</v>
       </c>
       <c r="V16" t="n">
-        <v>48.56100000000001</v>
+        <v>39.22959999999998</v>
       </c>
       <c r="W16" t="n">
-        <v>1.296418142421229</v>
+        <v>0.2061552812812452</v>
       </c>
       <c r="X16" t="n">
         <v>0</v>
@@ -3590,55 +3593,55 @@
     </row>
     <row r="17" spans="1:24">
       <c r="A17" s="2" t="n">
-        <v>569159</v>
+        <v>485334</v>
       </c>
       <c r="B17" t="n">
-        <v>46.02</v>
+        <v>41.05</v>
       </c>
       <c r="C17" t="n">
-        <v>46.3</v>
+        <v>41.1</v>
       </c>
       <c r="D17" t="n">
-        <v>45.27</v>
+        <v>40.51</v>
       </c>
       <c r="E17" t="n">
-        <v>45.31</v>
+        <v>40.76</v>
       </c>
       <c r="F17" t="n">
-        <v>4601233</v>
+        <v>7195205</v>
       </c>
       <c r="G17" t="n">
         <v>2017</v>
       </c>
       <c r="H17" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I17" t="n">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="J17" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17" t="n">
-        <v>-0.4659122872197338</v>
+        <v>0.05730274105886912</v>
       </c>
       <c r="M17" t="n">
-        <v>1.432743699760834</v>
+        <v>3.856706013166916</v>
       </c>
       <c r="N17" t="n">
-        <v>1.029999999999994</v>
+        <v>0.5900000000000034</v>
       </c>
       <c r="O17" t="n">
-        <v>0.03999999999999915</v>
+        <v>0.25</v>
       </c>
       <c r="P17" t="n">
-        <v>0.9899999999999949</v>
+        <v>0.3400000000000034</v>
       </c>
       <c r="Q17" t="n">
-        <v>-0.0149999999999999</v>
+        <v>-0.003422982885085579</v>
       </c>
       <c r="R17" t="b">
         <v>0</v>
@@ -3647,16 +3650,16 @@
         <v>0</v>
       </c>
       <c r="T17" t="n">
-        <v>45.23200000000006</v>
+        <v>40.62600000000003</v>
       </c>
       <c r="U17" t="n">
-        <v>44.97300000000003</v>
+        <v>39.51649999999998</v>
       </c>
       <c r="V17" t="n">
-        <v>48.4066</v>
+        <v>39.27719999999997</v>
       </c>
       <c r="W17" t="n">
-        <v>1.075360404701085</v>
+        <v>0.2085437033109019</v>
       </c>
       <c r="X17" t="n">
         <v>0</v>
@@ -3664,55 +3667,55 @@
     </row>
     <row r="18" spans="1:24">
       <c r="A18" s="2" t="n">
-        <v>569893</v>
+        <v>485381</v>
       </c>
       <c r="B18" t="n">
-        <v>45.28</v>
+        <v>40.64</v>
       </c>
       <c r="C18" t="n">
-        <v>45.66</v>
+        <v>40.73</v>
       </c>
       <c r="D18" t="n">
-        <v>44.03</v>
+        <v>40.24</v>
       </c>
       <c r="E18" t="n">
-        <v>44.38</v>
+        <v>40.4</v>
       </c>
       <c r="F18" t="n">
-        <v>6884589</v>
+        <v>7160171</v>
       </c>
       <c r="G18" t="n">
         <v>2017</v>
       </c>
       <c r="H18" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I18" t="n">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="J18" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K18" t="n">
         <v>0</v>
       </c>
       <c r="L18" t="n">
-        <v>-1.285691923486875</v>
+        <v>-0.4231299442879697</v>
       </c>
       <c r="M18" t="n">
-        <v>2.61105146450619</v>
+        <v>0.8615545899753888</v>
       </c>
       <c r="N18" t="n">
-        <v>1.629999999999995</v>
+        <v>0.4899999999999949</v>
       </c>
       <c r="O18" t="n">
-        <v>0.3500000000000014</v>
+        <v>0.1599999999999966</v>
       </c>
       <c r="P18" t="n">
-        <v>1.279999999999994</v>
+        <v>0.3299999999999983</v>
       </c>
       <c r="Q18" t="n">
-        <v>-0.02052527035974394</v>
+        <v>-0.008832188420019649</v>
       </c>
       <c r="R18" t="b">
         <v>0</v>
@@ -3721,16 +3724,16 @@
         <v>0</v>
       </c>
       <c r="T18" t="n">
-        <v>45.27800000000006</v>
+        <v>40.73000000000003</v>
       </c>
       <c r="U18" t="n">
-        <v>44.90650000000002</v>
+        <v>39.61949999999997</v>
       </c>
       <c r="V18" t="n">
-        <v>48.24100000000001</v>
+        <v>39.30339999999998</v>
       </c>
       <c r="W18" t="n">
-        <v>0.8272329089882425</v>
+        <v>0.2829857812348497</v>
       </c>
       <c r="X18" t="n">
         <v>0</v>
@@ -3738,73 +3741,73 @@
     </row>
     <row r="19" spans="1:24">
       <c r="A19" s="2" t="n">
-        <v>570309</v>
+        <v>486280</v>
       </c>
       <c r="B19" t="n">
-        <v>44.92</v>
+        <v>40.51</v>
       </c>
       <c r="C19" t="n">
-        <v>45.56</v>
+        <v>40.77</v>
       </c>
       <c r="D19" t="n">
-        <v>44.46</v>
+        <v>40.345</v>
       </c>
       <c r="E19" t="n">
-        <v>45.42</v>
+        <v>40.46</v>
       </c>
       <c r="F19" t="n">
-        <v>4708125</v>
+        <v>5908000</v>
       </c>
       <c r="G19" t="n">
         <v>2017</v>
       </c>
       <c r="H19" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I19" t="n">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="J19" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19" t="n">
-        <v>-0.4683234426527843</v>
+        <v>-0.6276525260843383</v>
       </c>
       <c r="M19" t="n">
-        <v>2.045164955593243</v>
+        <v>3.072813068168168</v>
       </c>
       <c r="N19" t="n">
-        <v>1.100000000000001</v>
+        <v>0.4250000000000043</v>
       </c>
       <c r="O19" t="n">
-        <v>0.9600000000000009</v>
+        <v>0.115000000000002</v>
       </c>
       <c r="P19" t="n">
-        <v>0.1400000000000006</v>
+        <v>0.3100000000000023</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.0234339792699414</v>
+        <v>0.001485148514851486</v>
       </c>
       <c r="R19" t="b">
         <v>1</v>
       </c>
       <c r="S19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T19" t="n">
-        <v>45.38900000000006</v>
+        <v>40.80600000000003</v>
       </c>
       <c r="U19" t="n">
-        <v>44.90700000000002</v>
+        <v>39.73299999999998</v>
       </c>
       <c r="V19" t="n">
-        <v>48.11720000000001</v>
+        <v>39.31539999999998</v>
       </c>
       <c r="W19" t="n">
-        <v>0.8439081421457111</v>
+        <v>0.2487971060927713</v>
       </c>
       <c r="X19" t="n">
         <v>0</v>
@@ -3812,73 +3815,73 @@
     </row>
     <row r="20" spans="1:24">
       <c r="A20" s="2" t="n">
-        <v>570919</v>
+        <v>486524</v>
       </c>
       <c r="B20" t="n">
-        <v>45.47</v>
+        <v>40.32</v>
       </c>
       <c r="C20" t="n">
-        <v>46.57</v>
+        <v>40.545</v>
       </c>
       <c r="D20" t="n">
-        <v>44.99</v>
+        <v>40.2</v>
       </c>
       <c r="E20" t="n">
-        <v>46.29</v>
+        <v>40.34</v>
       </c>
       <c r="F20" t="n">
-        <v>5864367</v>
+        <v>7351854</v>
       </c>
       <c r="G20" t="n">
         <v>2017</v>
       </c>
       <c r="H20" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I20" t="n">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="J20" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20" t="n">
-        <v>-1.474628043430845</v>
+        <v>-0.7890431174720585</v>
       </c>
       <c r="M20" t="n">
-        <v>2.589993880138018</v>
+        <v>1.616823599269708</v>
       </c>
       <c r="N20" t="n">
-        <v>1.579999999999998</v>
+        <v>0.3449999999999989</v>
       </c>
       <c r="O20" t="n">
-        <v>1.299999999999997</v>
+        <v>0.1400000000000006</v>
       </c>
       <c r="P20" t="n">
-        <v>0.2800000000000011</v>
+        <v>0.2049999999999983</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.01915455746367223</v>
+        <v>-0.002965892239248591</v>
       </c>
       <c r="R20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T20" t="n">
-        <v>45.63400000000006</v>
+        <v>40.76200000000002</v>
       </c>
       <c r="U20" t="n">
-        <v>45.02300000000002</v>
+        <v>39.83799999999998</v>
       </c>
       <c r="V20" t="n">
-        <v>47.96700000000001</v>
+        <v>39.32559999999998</v>
       </c>
       <c r="W20" t="n">
-        <v>0.8439081421457111</v>
+        <v>0.242339785071911</v>
       </c>
       <c r="X20" t="n">
         <v>0</v>
@@ -3886,73 +3889,73 @@
     </row>
     <row r="21" spans="1:24">
       <c r="A21" s="2" t="n">
-        <v>571469</v>
+        <v>487344</v>
       </c>
       <c r="B21" t="n">
-        <v>46.57</v>
+        <v>40.32</v>
       </c>
       <c r="C21" t="n">
-        <v>47.46</v>
+        <v>40.5</v>
       </c>
       <c r="D21" t="n">
-        <v>46.35</v>
+        <v>40.12</v>
       </c>
       <c r="E21" t="n">
-        <v>47.06</v>
+        <v>40.31</v>
       </c>
       <c r="F21" t="n">
-        <v>5342021</v>
+        <v>7773693</v>
       </c>
       <c r="G21" t="n">
         <v>2017</v>
       </c>
       <c r="H21" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I21" t="n">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="J21" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L21" t="n">
-        <v>-1.333277256461853</v>
+        <v>0.1047818358582695</v>
       </c>
       <c r="M21" t="n">
-        <v>2.922716300883411</v>
+        <v>4.2837991345131</v>
       </c>
       <c r="N21" t="n">
-        <v>1.109999999999999</v>
+        <v>0.3800000000000026</v>
       </c>
       <c r="O21" t="n">
-        <v>0.7100000000000009</v>
+        <v>0.1900000000000048</v>
       </c>
       <c r="P21" t="n">
-        <v>0.3999999999999986</v>
+        <v>0.1899999999999977</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.01663426225966735</v>
+        <v>-0.0007436787307882886</v>
       </c>
       <c r="R21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T21" t="n">
-        <v>45.98000000000006</v>
+        <v>40.71900000000002</v>
       </c>
       <c r="U21" t="n">
-        <v>45.23000000000003</v>
+        <v>39.93899999999999</v>
       </c>
       <c r="V21" t="n">
-        <v>47.83200000000001</v>
+        <v>39.33039999999998</v>
       </c>
       <c r="W21" t="n">
-        <v>0.8583261673295779</v>
+        <v>0.269063632056363</v>
       </c>
       <c r="X21" t="n">
         <v>0</v>
@@ -3960,73 +3963,73 @@
     </row>
     <row r="22" spans="1:24">
       <c r="A22" s="2" t="n">
-        <v>571680</v>
+        <v>487669</v>
       </c>
       <c r="B22" t="n">
-        <v>46.98</v>
+        <v>39.76</v>
       </c>
       <c r="C22" t="n">
-        <v>47.96</v>
+        <v>40.465</v>
       </c>
       <c r="D22" t="n">
-        <v>46.89</v>
+        <v>39.25</v>
       </c>
       <c r="E22" t="n">
-        <v>47.7</v>
+        <v>40.31</v>
       </c>
       <c r="F22" t="n">
-        <v>6363180</v>
+        <v>16890214</v>
       </c>
       <c r="G22" t="n">
         <v>2017</v>
       </c>
       <c r="H22" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I22" t="n">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="J22" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L22" t="n">
-        <v>-0.006269613013595374</v>
+        <v>-1.029016761934884</v>
       </c>
       <c r="M22" t="n">
-        <v>1.291132569398427</v>
+        <v>2.347719007881989</v>
       </c>
       <c r="N22" t="n">
-        <v>1.07</v>
+        <v>1.215000000000003</v>
       </c>
       <c r="O22" t="n">
-        <v>0.8100000000000023</v>
+        <v>1.060000000000002</v>
       </c>
       <c r="P22" t="n">
-        <v>0.259999999999998</v>
+        <v>0.1550000000000011</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.01359966000849977</v>
+        <v>0</v>
       </c>
       <c r="R22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T22" t="n">
-        <v>46.16400000000006</v>
+        <v>40.62100000000002</v>
       </c>
       <c r="U22" t="n">
-        <v>45.35250000000003</v>
+        <v>40.03349999999999</v>
       </c>
       <c r="V22" t="n">
-        <v>47.70160000000001</v>
+        <v>39.32439999999998</v>
       </c>
       <c r="W22" t="n">
-        <v>1.120337959214088</v>
+        <v>0.2369749836106363</v>
       </c>
       <c r="X22" t="n">
         <v>0</v>
@@ -4034,73 +4037,73 @@
     </row>
     <row r="23" spans="1:24">
       <c r="A23" s="2" t="n">
-        <v>572338</v>
+        <v>488227</v>
       </c>
       <c r="B23" t="n">
-        <v>47.84</v>
+        <v>40.46</v>
       </c>
       <c r="C23" t="n">
-        <v>48.26</v>
+        <v>41.12</v>
       </c>
       <c r="D23" t="n">
-        <v>47.23</v>
+        <v>40.45</v>
       </c>
       <c r="E23" t="n">
-        <v>47.58</v>
+        <v>40.96</v>
       </c>
       <c r="F23" t="n">
-        <v>4706004</v>
+        <v>9410238</v>
       </c>
       <c r="G23" t="n">
         <v>2017</v>
       </c>
       <c r="H23" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I23" t="n">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="J23" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K23" t="n">
         <v>0</v>
       </c>
       <c r="L23" t="n">
-        <v>-0.9134282951663728</v>
+        <v>-0.9127689125423583</v>
       </c>
       <c r="M23" t="n">
-        <v>2.036878823044319</v>
+        <v>2.820585332886515</v>
       </c>
       <c r="N23" t="n">
-        <v>1.030000000000001</v>
+        <v>0.6699999999999946</v>
       </c>
       <c r="O23" t="n">
-        <v>0.3500000000000014</v>
+        <v>0.509999999999998</v>
       </c>
       <c r="P23" t="n">
-        <v>0.6799999999999997</v>
+        <v>0.1599999999999966</v>
       </c>
       <c r="Q23" t="n">
-        <v>-0.002515723270440362</v>
+        <v>0.01612503100967499</v>
       </c>
       <c r="R23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S23" t="b">
         <v>1</v>
       </c>
       <c r="T23" t="n">
-        <v>46.29300000000005</v>
+        <v>40.60900000000002</v>
       </c>
       <c r="U23" t="n">
-        <v>45.48400000000002</v>
+        <v>40.15149999999998</v>
       </c>
       <c r="V23" t="n">
-        <v>47.57580000000001</v>
+        <v>39.34079999999997</v>
       </c>
       <c r="W23" t="n">
-        <v>1.264811297801546</v>
+        <v>0.2544181035789138</v>
       </c>
       <c r="X23" t="n">
         <v>0</v>
@@ -4108,73 +4111,73 @@
     </row>
     <row r="24" spans="1:24">
       <c r="A24" s="2" t="n">
-        <v>572797</v>
+        <v>488825</v>
       </c>
       <c r="B24" t="n">
-        <v>47.58</v>
+        <v>41.11</v>
       </c>
       <c r="C24" t="n">
-        <v>48.1</v>
+        <v>41.31</v>
       </c>
       <c r="D24" t="n">
-        <v>46.6301</v>
+        <v>40.9</v>
       </c>
       <c r="E24" t="n">
-        <v>46.85</v>
+        <v>41</v>
       </c>
       <c r="F24" t="n">
-        <v>6183158</v>
+        <v>7033637</v>
       </c>
       <c r="G24" t="n">
         <v>2017</v>
       </c>
       <c r="H24" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I24" t="n">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="J24" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24" t="n">
-        <v>-0.8477856206627032</v>
+        <v>0.3288428777494597</v>
       </c>
       <c r="M24" t="n">
-        <v>1.94280893986287</v>
+        <v>3.480462443956647</v>
       </c>
       <c r="N24" t="n">
-        <v>1.469900000000003</v>
+        <v>0.4100000000000037</v>
       </c>
       <c r="O24" t="n">
-        <v>0.2199000000000026</v>
+        <v>0.1000000000000014</v>
       </c>
       <c r="P24" t="n">
-        <v>1.25</v>
+        <v>0.3100000000000023</v>
       </c>
       <c r="Q24" t="n">
-        <v>-0.01534258091635132</v>
+        <v>0.0009765625</v>
       </c>
       <c r="R24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T24" t="n">
-        <v>46.27800000000006</v>
+        <v>40.63700000000002</v>
       </c>
       <c r="U24" t="n">
-        <v>45.59850000000002</v>
+        <v>40.29049999999999</v>
       </c>
       <c r="V24" t="n">
-        <v>47.4498</v>
+        <v>39.37679999999997</v>
       </c>
       <c r="W24" t="n">
-        <v>1.206958002188313</v>
+        <v>0.3054504869862245</v>
       </c>
       <c r="X24" t="n">
         <v>0</v>
@@ -4182,73 +4185,73 @@
     </row>
     <row r="25" spans="1:24">
       <c r="A25" s="2" t="n">
-        <v>573131</v>
+        <v>489051</v>
       </c>
       <c r="B25" t="n">
-        <v>46.78</v>
+        <v>40.86</v>
       </c>
       <c r="C25" t="n">
-        <v>48.6</v>
+        <v>41.14</v>
       </c>
       <c r="D25" t="n">
-        <v>46.78</v>
+        <v>40.77</v>
       </c>
       <c r="E25" t="n">
-        <v>47.49</v>
+        <v>41.01</v>
       </c>
       <c r="F25" t="n">
-        <v>8367839</v>
+        <v>13811560</v>
       </c>
       <c r="G25" t="n">
         <v>2017</v>
       </c>
       <c r="H25" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I25" t="n">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="J25" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L25" t="n">
-        <v>0.02020700468688488</v>
+        <v>-1.02080231377101</v>
       </c>
       <c r="M25" t="n">
-        <v>0.6303744980404227</v>
+        <v>1.721756715354916</v>
       </c>
       <c r="N25" t="n">
-        <v>1.82</v>
+        <v>0.3699999999999974</v>
       </c>
       <c r="O25" t="n">
-        <v>0.7100000000000009</v>
+        <v>0.2399999999999949</v>
       </c>
       <c r="P25" t="n">
-        <v>1.109999999999999</v>
+        <v>0.1300000000000026</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.01366061899679827</v>
+        <v>0.0002439024390243905</v>
       </c>
       <c r="R25" t="b">
         <v>1</v>
       </c>
       <c r="S25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T25" t="n">
-        <v>46.40800000000006</v>
+        <v>40.64500000000002</v>
       </c>
       <c r="U25" t="n">
-        <v>45.75700000000002</v>
+        <v>40.42549999999999</v>
       </c>
       <c r="V25" t="n">
-        <v>47.3474</v>
+        <v>39.40079999999998</v>
       </c>
       <c r="W25" t="n">
-        <v>0.8205631051433722</v>
+        <v>0.3434974180261089</v>
       </c>
       <c r="X25" t="n">
         <v>0</v>
@@ -4256,73 +4259,73 @@
     </row>
     <row r="26" spans="1:24">
       <c r="A26" s="2" t="n">
-        <v>573928</v>
+        <v>489604</v>
       </c>
       <c r="B26" t="n">
-        <v>47.49</v>
+        <v>40.73</v>
       </c>
       <c r="C26" t="n">
-        <v>47.85</v>
+        <v>41.79</v>
       </c>
       <c r="D26" t="n">
-        <v>47.23</v>
+        <v>40.6</v>
       </c>
       <c r="E26" t="n">
-        <v>47.49</v>
+        <v>41.77</v>
       </c>
       <c r="F26" t="n">
-        <v>4904347</v>
+        <v>12318224</v>
       </c>
       <c r="G26" t="n">
         <v>2017</v>
       </c>
       <c r="H26" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I26" t="n">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="J26" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L26" t="n">
-        <v>-0.01504730585650039</v>
+        <v>-0.8828431235293814</v>
       </c>
       <c r="M26" t="n">
-        <v>2.487928081791531</v>
+        <v>2.015023563937461</v>
       </c>
       <c r="N26" t="n">
-        <v>0.6200000000000045</v>
+        <v>1.189999999999998</v>
       </c>
       <c r="O26" t="n">
-        <v>0.2600000000000051</v>
+        <v>1.170000000000002</v>
       </c>
       <c r="P26" t="n">
-        <v>0.3599999999999994</v>
+        <v>0.01999999999999602</v>
       </c>
       <c r="Q26" t="n">
-        <v>0</v>
+        <v>0.01853206534991481</v>
       </c>
       <c r="R26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S26" t="b">
         <v>1</v>
       </c>
       <c r="T26" t="n">
-        <v>46.55700000000006</v>
+        <v>40.73200000000002</v>
       </c>
       <c r="U26" t="n">
-        <v>45.89450000000002</v>
+        <v>40.59349999999999</v>
       </c>
       <c r="V26" t="n">
-        <v>47.25039999999999</v>
+        <v>39.43719999999998</v>
       </c>
       <c r="W26" t="n">
-        <v>0.5053523052085895</v>
+        <v>0.5386667845357113</v>
       </c>
       <c r="X26" t="n">
         <v>0</v>
@@ -4330,55 +4333,55 @@
     </row>
     <row r="27" spans="1:24">
       <c r="A27" s="2" t="n">
-        <v>574386</v>
+        <v>490087</v>
       </c>
       <c r="B27" t="n">
-        <v>47.52</v>
+        <v>41.51</v>
       </c>
       <c r="C27" t="n">
-        <v>47.93</v>
+        <v>42.37</v>
       </c>
       <c r="D27" t="n">
-        <v>47.22</v>
+        <v>41.44</v>
       </c>
       <c r="E27" t="n">
-        <v>47.73</v>
+        <v>42.33</v>
       </c>
       <c r="F27" t="n">
-        <v>4911650</v>
+        <v>11948793</v>
       </c>
       <c r="G27" t="n">
         <v>2017</v>
       </c>
       <c r="H27" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I27" t="n">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="J27" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L27" t="n">
-        <v>0.3757415577021215</v>
+        <v>-0.1093214771245346</v>
       </c>
       <c r="M27" t="n">
-        <v>2.296855841165298</v>
+        <v>1.876095384361021</v>
       </c>
       <c r="N27" t="n">
-        <v>0.7100000000000009</v>
+        <v>0.9299999999999997</v>
       </c>
       <c r="O27" t="n">
-        <v>0.509999999999998</v>
+        <v>0.8900000000000006</v>
       </c>
       <c r="P27" t="n">
-        <v>0.2000000000000028</v>
+        <v>0.03999999999999915</v>
       </c>
       <c r="Q27" t="n">
-        <v>0.005053695514845025</v>
+        <v>0.01340675125688273</v>
       </c>
       <c r="R27" t="b">
         <v>1</v>
@@ -4387,16 +4390,16 @@
         <v>1</v>
       </c>
       <c r="T27" t="n">
-        <v>46.79900000000005</v>
+        <v>40.88900000000002</v>
       </c>
       <c r="U27" t="n">
-        <v>46.01550000000002</v>
+        <v>40.75749999999999</v>
       </c>
       <c r="V27" t="n">
-        <v>47.16679999999999</v>
+        <v>39.47599999999997</v>
       </c>
       <c r="W27" t="n">
-        <v>0.3327089390050966</v>
+        <v>0.7357179842719007</v>
       </c>
       <c r="X27" t="n">
         <v>0</v>
@@ -4404,55 +4407,55 @@
     </row>
     <row r="28" spans="1:24">
       <c r="A28" s="2" t="n">
-        <v>575133</v>
+        <v>490835</v>
       </c>
       <c r="B28" t="n">
-        <v>47.66</v>
+        <v>42.18</v>
       </c>
       <c r="C28" t="n">
-        <v>50.59</v>
+        <v>42.79</v>
       </c>
       <c r="D28" t="n">
-        <v>47.63</v>
+        <v>41.85</v>
       </c>
       <c r="E28" t="n">
-        <v>50.51</v>
+        <v>42.75</v>
       </c>
       <c r="F28" t="n">
-        <v>10261794</v>
+        <v>11836897</v>
       </c>
       <c r="G28" t="n">
         <v>2017</v>
       </c>
       <c r="H28" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I28" t="n">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="J28" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K28" t="n">
         <v>0</v>
       </c>
       <c r="L28" t="n">
-        <v>-0.6009207384725234</v>
+        <v>-0.7993494471092238</v>
       </c>
       <c r="M28" t="n">
-        <v>6.175202707381984</v>
+        <v>3.547472743112887</v>
       </c>
       <c r="N28" t="n">
-        <v>2.960000000000001</v>
+        <v>0.9399999999999977</v>
       </c>
       <c r="O28" t="n">
-        <v>2.879999999999995</v>
+        <v>0.8999999999999986</v>
       </c>
       <c r="P28" t="n">
-        <v>0.0800000000000054</v>
+        <v>0.03999999999999915</v>
       </c>
       <c r="Q28" t="n">
-        <v>0.05824429080243032</v>
+        <v>0.009922041105598911</v>
       </c>
       <c r="R28" t="b">
         <v>1</v>
@@ -4461,16 +4464,16 @@
         <v>1</v>
       </c>
       <c r="T28" t="n">
-        <v>47.41200000000006</v>
+        <v>41.12400000000002</v>
       </c>
       <c r="U28" t="n">
-        <v>46.34500000000002</v>
+        <v>40.92699999999999</v>
       </c>
       <c r="V28" t="n">
-        <v>47.1514</v>
+        <v>39.53419999999997</v>
       </c>
       <c r="W28" t="n">
-        <v>1.18474630597542</v>
+        <v>0.8662700557701316</v>
       </c>
       <c r="X28" t="n">
         <v>0</v>
@@ -4478,55 +4481,55 @@
     </row>
     <row r="29" spans="1:24">
       <c r="A29" s="2" t="n">
-        <v>575287</v>
+        <v>491077</v>
       </c>
       <c r="B29" t="n">
-        <v>50.5</v>
+        <v>42.94</v>
       </c>
       <c r="C29" t="n">
-        <v>51.67</v>
+        <v>43.13</v>
       </c>
       <c r="D29" t="n">
-        <v>50.49</v>
+        <v>42.54</v>
       </c>
       <c r="E29" t="n">
-        <v>50.73</v>
+        <v>42.78</v>
       </c>
       <c r="F29" t="n">
-        <v>7454460</v>
+        <v>11642218</v>
       </c>
       <c r="G29" t="n">
         <v>2017</v>
       </c>
       <c r="H29" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I29" t="n">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="J29" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L29" t="n">
-        <v>-0.02395674022380025</v>
+        <v>-1.187355840748546</v>
       </c>
       <c r="M29" t="n">
-        <v>1.658308543605768</v>
+        <v>1.888685359692112</v>
       </c>
       <c r="N29" t="n">
-        <v>1.18</v>
+        <v>0.5900000000000034</v>
       </c>
       <c r="O29" t="n">
-        <v>0.2399999999999949</v>
+        <v>0.240000000000002</v>
       </c>
       <c r="P29" t="n">
-        <v>0.9400000000000048</v>
+        <v>0.3500000000000014</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.004355573153830949</v>
+        <v>0.0007017543859648701</v>
       </c>
       <c r="R29" t="b">
         <v>1</v>
@@ -4535,16 +4538,16 @@
         <v>1</v>
       </c>
       <c r="T29" t="n">
-        <v>47.94300000000005</v>
+        <v>41.35600000000002</v>
       </c>
       <c r="U29" t="n">
-        <v>46.66600000000002</v>
+        <v>41.08099999999999</v>
       </c>
       <c r="V29" t="n">
-        <v>47.15379999999999</v>
+        <v>39.59459999999997</v>
       </c>
       <c r="W29" t="n">
-        <v>1.583024531289773</v>
+        <v>0.8280901722237356</v>
       </c>
       <c r="X29" t="n">
         <v>0</v>
@@ -4552,73 +4555,73 @@
     </row>
     <row r="30" spans="1:24">
       <c r="A30" s="2" t="n">
-        <v>576035</v>
+        <v>491770</v>
       </c>
       <c r="B30" t="n">
-        <v>50.85</v>
+        <v>42.57</v>
       </c>
       <c r="C30" t="n">
-        <v>50.99</v>
+        <v>42.75</v>
       </c>
       <c r="D30" t="n">
-        <v>50.26</v>
+        <v>42.23</v>
       </c>
       <c r="E30" t="n">
-        <v>50.56</v>
+        <v>42.43</v>
       </c>
       <c r="F30" t="n">
-        <v>4212310</v>
+        <v>8735171</v>
       </c>
       <c r="G30" t="n">
         <v>2017</v>
       </c>
       <c r="H30" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I30" t="n">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="J30" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L30" t="n">
-        <v>-0.08034694571172228</v>
+        <v>-0.5903496959107986</v>
       </c>
       <c r="M30" t="n">
-        <v>3.073045456024727</v>
+        <v>3.090394935894819</v>
       </c>
       <c r="N30" t="n">
-        <v>0.730000000000004</v>
+        <v>0.5200000000000031</v>
       </c>
       <c r="O30" t="n">
-        <v>0.3000000000000043</v>
+        <v>0.2000000000000028</v>
       </c>
       <c r="P30" t="n">
-        <v>0.4299999999999997</v>
+        <v>0.3200000000000003</v>
       </c>
       <c r="Q30" t="n">
-        <v>-0.003351074315000924</v>
+        <v>-0.008181393174380602</v>
       </c>
       <c r="R30" t="b">
         <v>0</v>
       </c>
       <c r="S30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T30" t="n">
-        <v>48.37000000000005</v>
+        <v>41.56500000000002</v>
       </c>
       <c r="U30" t="n">
-        <v>47.00200000000002</v>
+        <v>41.16349999999998</v>
       </c>
       <c r="V30" t="n">
-        <v>47.14479999999999</v>
+        <v>39.68119999999998</v>
       </c>
       <c r="W30" t="n">
-        <v>1.737717441001381</v>
+        <v>0.7634352188192198</v>
       </c>
       <c r="X30" t="n">
         <v>0</v>
@@ -4626,55 +4629,55 @@
     </row>
     <row r="31" spans="1:24">
       <c r="A31" s="2" t="n">
-        <v>576518</v>
+        <v>492283</v>
       </c>
       <c r="B31" t="n">
-        <v>50.7</v>
+        <v>42.57</v>
       </c>
       <c r="C31" t="n">
-        <v>51.59</v>
+        <v>42.98</v>
       </c>
       <c r="D31" t="n">
-        <v>50.65</v>
+        <v>42.504</v>
       </c>
       <c r="E31" t="n">
-        <v>51.3</v>
+        <v>42.89</v>
       </c>
       <c r="F31" t="n">
-        <v>4240506</v>
+        <v>8697290</v>
       </c>
       <c r="G31" t="n">
         <v>2017</v>
       </c>
       <c r="H31" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I31" t="n">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="J31" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L31" t="n">
-        <v>0.4915200048718373</v>
+        <v>-0.4503729386714377</v>
       </c>
       <c r="M31" t="n">
-        <v>2.94253478317885</v>
+        <v>3.320899223735304</v>
       </c>
       <c r="N31" t="n">
-        <v>0.9400000000000048</v>
+        <v>0.4759999999999991</v>
       </c>
       <c r="O31" t="n">
-        <v>0.6499999999999986</v>
+        <v>0.3860000000000028</v>
       </c>
       <c r="P31" t="n">
-        <v>0.2900000000000063</v>
+        <v>0.08999999999999631</v>
       </c>
       <c r="Q31" t="n">
-        <v>0.01463607594936689</v>
+        <v>0.01084138581192562</v>
       </c>
       <c r="R31" t="b">
         <v>1</v>
@@ -4683,16 +4686,16 @@
         <v>1</v>
       </c>
       <c r="T31" t="n">
-        <v>48.79400000000005</v>
+        <v>41.82300000000002</v>
       </c>
       <c r="U31" t="n">
-        <v>47.38700000000001</v>
+        <v>41.27099999999999</v>
       </c>
       <c r="V31" t="n">
-        <v>47.17079999999999</v>
+        <v>39.75939999999998</v>
       </c>
       <c r="W31" t="n">
-        <v>1.734055252593186</v>
+        <v>0.6758944690804717</v>
       </c>
       <c r="X31" t="n">
         <v>0</v>
@@ -4724,7 +4727,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="n">
-        <v>561663</v>
+        <v>477829</v>
       </c>
       <c r="B2" t="n">
         <v>2</v>
@@ -4732,31 +4735,31 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="n">
-        <v>562220</v>
+        <v>477914</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="n">
-        <v>562614</v>
+        <v>478690</v>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="n">
-        <v>563204</v>
+        <v>479104</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="n">
-        <v>563647</v>
+        <v>479383</v>
       </c>
       <c r="B6" t="n">
         <v>2</v>
@@ -4764,7 +4767,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="n">
-        <v>564452</v>
+        <v>479880</v>
       </c>
       <c r="B7" t="n">
         <v>2</v>
@@ -4772,15 +4775,15 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="n">
-        <v>564990</v>
+        <v>480634</v>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="n">
-        <v>565558</v>
+        <v>481023</v>
       </c>
       <c r="B9" t="n">
         <v>2</v>
@@ -4788,15 +4791,15 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="n">
-        <v>565958</v>
+        <v>481465</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="n">
-        <v>566066</v>
+        <v>481988</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
@@ -4804,7 +4807,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="n">
-        <v>567055</v>
+        <v>482798</v>
       </c>
       <c r="B12" t="n">
         <v>2</v>
@@ -4812,7 +4815,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="n">
-        <v>567285</v>
+        <v>483171</v>
       </c>
       <c r="B13" t="n">
         <v>2</v>
@@ -4820,23 +4823,23 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="n">
-        <v>567852</v>
+        <v>483525</v>
       </c>
       <c r="B14" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2" t="n">
-        <v>568132</v>
+        <v>484129</v>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2" t="n">
-        <v>569058</v>
+        <v>484770</v>
       </c>
       <c r="B16" t="n">
         <v>2</v>
@@ -4844,7 +4847,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2" t="n">
-        <v>569159</v>
+        <v>485334</v>
       </c>
       <c r="B17" t="n">
         <v>0</v>
@@ -4852,7 +4855,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2" t="n">
-        <v>569893</v>
+        <v>485381</v>
       </c>
       <c r="B18" t="n">
         <v>0</v>
@@ -4860,15 +4863,15 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2" t="n">
-        <v>570309</v>
+        <v>486280</v>
       </c>
       <c r="B19" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="n">
-        <v>570919</v>
+        <v>486524</v>
       </c>
       <c r="B20" t="n">
         <v>2</v>
@@ -4876,15 +4879,15 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2" t="n">
-        <v>571469</v>
+        <v>487344</v>
       </c>
       <c r="B21" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2" t="n">
-        <v>571680</v>
+        <v>487669</v>
       </c>
       <c r="B22" t="n">
         <v>2</v>
@@ -4892,15 +4895,15 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2" t="n">
-        <v>572338</v>
+        <v>488227</v>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2" t="n">
-        <v>572797</v>
+        <v>488825</v>
       </c>
       <c r="B24" t="n">
         <v>0</v>
@@ -4908,7 +4911,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2" t="n">
-        <v>573131</v>
+        <v>489051</v>
       </c>
       <c r="B25" t="n">
         <v>2</v>
@@ -4916,15 +4919,15 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2" t="n">
-        <v>573928</v>
+        <v>489604</v>
       </c>
       <c r="B26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2" t="n">
-        <v>574386</v>
+        <v>490087</v>
       </c>
       <c r="B27" t="n">
         <v>2</v>
@@ -4932,7 +4935,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2" t="n">
-        <v>575133</v>
+        <v>490835</v>
       </c>
       <c r="B28" t="n">
         <v>2</v>
@@ -4940,15 +4943,15 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2" t="n">
-        <v>575287</v>
+        <v>491077</v>
       </c>
       <c r="B29" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2" t="n">
-        <v>576035</v>
+        <v>491770</v>
       </c>
       <c r="B30" t="n">
         <v>0</v>
@@ -4956,7 +4959,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2" t="n">
-        <v>576518</v>
+        <v>492283</v>
       </c>
       <c r="B31" t="n">
         <v>2</v>
@@ -4973,7 +4976,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5000,10 +5003,10 @@
         <v>70</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5</v>
+        <v>0.4776119402985075</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3385315183102968</v>
+        <v>0.3430030270447529</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5014,10 +5017,10 @@
         <v>71</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8358974358974359</v>
+        <v>0.8253731343283581</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6171475994429033</v>
+        <v>0.6115162479943878</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5028,10 +5031,10 @@
         <v>72</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.7671641791044777</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6143746307616379</v>
+        <v>0.5663965156577269</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -5042,10 +5045,10 @@
         <v>73</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8423076923076923</v>
+        <v>0.7970149253731342</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6208436510746038</v>
+        <v>0.5923596439124234</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -5056,10 +5059,10 @@
         <v>74</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8294871794871795</v>
+        <v>0.8044776119402984</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6147684074332628</v>
+        <v>0.5977935660269174</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -5070,10 +5073,10 @@
         <v>75</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8435897435897435</v>
+        <v>0.7805970149253731</v>
       </c>
       <c r="D7" t="n">
-        <v>0.624086450913218</v>
+        <v>0.6072346892859561</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -5084,10 +5087,10 @@
         <v>76</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8615384615384615</v>
+        <v>0.8283582089552238</v>
       </c>
       <c r="D8" t="n">
-        <v>0.6308356966841436</v>
+        <v>0.6112040642913918</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -5098,10 +5101,24 @@
         <v>77</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8461538461538461</v>
+        <v>0.8223880597014924</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5678901200377122</v>
+        <v>0.6160127977022058</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.7208955223880597</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.5008222993043293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>